<commit_message>
Now loads basics for Troops from Excel.
</commit_message>
<xml_diff>
--- a/src/test/resources/sides.xlsx
+++ b/src/test/resources/sides.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="60" windowWidth="10500" windowHeight="6912"/>
+    <workbookView xWindow="192" yWindow="60" windowWidth="10500" windowHeight="6912" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sides" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Troops" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -25,6 +25,24 @@
   </si>
   <si>
     <t>Second Test Side</t>
+  </si>
+  <si>
+    <t>Side</t>
+  </si>
+  <si>
+    <t>Troop Count</t>
+  </si>
+  <si>
+    <t>Damage Dealt Per Troop</t>
+  </si>
+  <si>
+    <t>Hit Points Per Troop</t>
+  </si>
+  <si>
+    <t>First Test Side Troops</t>
+  </si>
+  <si>
+    <t>Second Test Side Troops</t>
   </si>
 </sst>
 </file>
@@ -375,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -407,13 +425,75 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="17.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1000</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>10000</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>